<commit_message>
imported new gifts app xlsx file
</commit_message>
<xml_diff>
--- a/assets/gifts app localization.xlsx
+++ b/assets/gifts app localization.xlsx
@@ -10,8 +10,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="B142">
+      <text>
+        <t xml:space="preserve">need to be set
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="660">
   <si>
     <t>localization_keys</t>
   </si>
@@ -34,7 +50,7 @@
     <t>تطبيق هدية</t>
   </si>
   <si>
-    <t>Geschenk App</t>
+    <t>Geschenke-App</t>
   </si>
   <si>
     <t>get_gifts</t>
@@ -43,16 +59,34 @@
     <t>Get Gifts</t>
   </si>
   <si>
+    <t>احصل على الهدايا</t>
+  </si>
+  <si>
+    <t>Geschenke bekommen</t>
+  </si>
+  <si>
     <t>play_games</t>
   </si>
   <si>
     <t>Play Games</t>
   </si>
   <si>
-    <t>earn_money</t>
-  </si>
-  <si>
-    <t>Earn Money</t>
+    <t>لعب الألعاب</t>
+  </si>
+  <si>
+    <t>Spiele spielen</t>
+  </si>
+  <si>
+    <t>various_awards</t>
+  </si>
+  <si>
+    <t>Various awards</t>
+  </si>
+  <si>
+    <t>جوائز متنوعة</t>
+  </si>
+  <si>
+    <t>Verschiedene Auszeichnungen</t>
   </si>
   <si>
     <t>intro_message1</t>
@@ -64,7 +98,7 @@
     <t>مع تطبيق هدية سوف تستثمر وقتك بالربح من هاتفك</t>
   </si>
   <si>
-    <t>Mit "Geschenke-App" investiere dein Zeit, um wertvolle Geschenke zu bekommen.</t>
+    <t>Mit "Gifts App" investierst du deine Zeit, um wertvolle Geschenke zu verdienen.</t>
   </si>
   <si>
     <t>intro_message2</t>
@@ -76,7 +110,7 @@
     <t>لاول مرة اجمع النقاط من كل دقيقة تلعب بها بالالعاب المفضلة لك</t>
   </si>
   <si>
-    <t>Du erhältst Münzen für jede Minute, die du spielst.</t>
+    <t>Für jede Minute, die du spielst, erhältst du Münzen.</t>
   </si>
   <si>
     <t>intro_message3</t>
@@ -88,7 +122,7 @@
     <t>بدل نقاطك بفلوس كاش او ببطاقات ببجي او بنقاط تيك توك و الكثير من الهدايا المميزة</t>
   </si>
   <si>
-    <t>Du kannst dein Geschenk aus vielen Geschenkkarten auswählen oder das Mobile aufladen oder Bargeld erhalten.</t>
+    <t>Sie können Ihr Geschenk aus vielen Geschenkkarten auswählen oder Ihr Handyguthaben aufladen oder Bargeld erhalten.</t>
   </si>
   <si>
     <t>next</t>
@@ -100,7 +134,7 @@
     <t>التالي</t>
   </si>
   <si>
-    <t>Nächste</t>
+    <t>Weiter</t>
   </si>
   <si>
     <t>lets_start</t>
@@ -112,160 +146,310 @@
     <t>هيا نبدأ</t>
   </si>
   <si>
+    <t>Los geht's</t>
+  </si>
+  <si>
     <t>log_in_message</t>
   </si>
   <si>
     <t>We make the login process very easy for you</t>
   </si>
   <si>
+    <t>جعلنا عملية التسجيل بسيطة من أجلك</t>
+  </si>
+  <si>
+    <t>Wir machen den Anmeldeprozess sehr einfach für Sie</t>
+  </si>
+  <si>
     <t>sign_in_with_google</t>
   </si>
   <si>
     <t>Sign in with google</t>
   </si>
   <si>
+    <t>تسجيل الدخول بإيميل جيميل</t>
+  </si>
+  <si>
+    <t>Mit Google anmelden</t>
+  </si>
+  <si>
     <t>data_collection_hint</t>
   </si>
   <si>
     <t>Why is collection data necessary?</t>
   </si>
   <si>
+    <t>لماذا جمع البيانات ضروري؟</t>
+  </si>
+  <si>
+    <t>Warum ist die Datenerfassung notwendig?</t>
+  </si>
+  <si>
     <t>continue</t>
   </si>
   <si>
     <t>Continue</t>
   </si>
   <si>
+    <t>متابعة</t>
+  </si>
+  <si>
     <t>agree_data_collect</t>
   </si>
   <si>
     <t>Agree all data collection</t>
   </si>
   <si>
+    <t>موافقة على جميع الشروط</t>
+  </si>
+  <si>
+    <t>Einverständnis zur Datenerfassung</t>
+  </si>
+  <si>
     <t>no_internet_connection</t>
   </si>
   <si>
     <t>Please connect to the internet</t>
   </si>
   <si>
+    <t>يرجى الاتصال بالانترنت</t>
+  </si>
+  <si>
+    <t>Bitte verbinden Sie sich mit dem Internet</t>
+  </si>
+  <si>
     <t>connection_error</t>
   </si>
   <si>
     <t>Connection error</t>
   </si>
   <si>
+    <t>خطأ في الاتصال</t>
+  </si>
+  <si>
+    <t>Verbindungsfehler</t>
+  </si>
+  <si>
     <t>all_games</t>
   </si>
   <si>
     <t>All games</t>
   </si>
   <si>
+    <t>جميع الألعاب</t>
+  </si>
+  <si>
+    <t>Alle Spiele</t>
+  </si>
+  <si>
     <t>play_time</t>
   </si>
   <si>
     <t>Play time</t>
   </si>
   <si>
+    <t>وقت اللعب</t>
+  </si>
+  <si>
+    <t>Spielzeit</t>
+  </si>
+  <si>
     <t>play</t>
   </si>
   <si>
     <t>Play</t>
   </si>
   <si>
+    <t>لعب</t>
+  </si>
+  <si>
+    <t>Spielen</t>
+  </si>
+  <si>
     <t>statistics</t>
   </si>
   <si>
     <t>Statistics</t>
   </si>
   <si>
+    <t>الإحصاءات</t>
+  </si>
+  <si>
+    <t>Statistik</t>
+  </si>
+  <si>
     <t>gifts</t>
   </si>
   <si>
     <t>Gifts</t>
   </si>
   <si>
+    <t>الهدايا</t>
+  </si>
+  <si>
+    <t>Geschenke</t>
+  </si>
+  <si>
     <t>settings</t>
   </si>
   <si>
     <t>Settings</t>
   </si>
   <si>
+    <t>الإعدادات</t>
+  </si>
+  <si>
+    <t>Einstellungen</t>
+  </si>
+  <si>
     <t>my_gifts</t>
   </si>
   <si>
     <t>My Gifts</t>
   </si>
   <si>
+    <t>جميع الهدايا</t>
+  </si>
+  <si>
+    <t>Meine Geschenke</t>
+  </si>
+  <si>
     <t>play_history</t>
   </si>
   <si>
     <t>Playtime history</t>
   </si>
   <si>
+    <t>سجل النقاط</t>
+  </si>
+  <si>
+    <t>Spielzeitverlauf</t>
+  </si>
+  <si>
     <t>top_10</t>
   </si>
   <si>
     <t>Top 10</t>
   </si>
   <si>
+    <t>توب 10</t>
+  </si>
+  <si>
     <t>winners_today</t>
   </si>
   <si>
     <t>Winners today</t>
   </si>
   <si>
+    <t>الرابحين اليوم</t>
+  </si>
+  <si>
+    <t>Gewinner heute</t>
+  </si>
+  <si>
     <t>language</t>
   </si>
   <si>
     <t>Language</t>
   </si>
   <si>
+    <t>اللغة</t>
+  </si>
+  <si>
+    <t>Sprache</t>
+  </si>
+  <si>
     <t>rate_app</t>
   </si>
   <si>
     <t>Rate gifts app</t>
   </si>
   <si>
+    <t>تقييم التطبيق</t>
+  </si>
+  <si>
+    <t>Geschenke-App bewerten</t>
+  </si>
+  <si>
     <t>share_app</t>
   </si>
   <si>
     <t>Share gifts app</t>
   </si>
   <si>
+    <t>مشاركة التطبيق</t>
+  </si>
+  <si>
+    <t>Geschenke-App teilen</t>
+  </si>
+  <si>
     <t>contact_us</t>
   </si>
   <si>
     <t>Contact with us</t>
   </si>
   <si>
+    <t>تواصل معنا</t>
+  </si>
+  <si>
+    <t>Kontakt mit uns</t>
+  </si>
+  <si>
     <t>common_questions</t>
   </si>
   <si>
     <t>FAQ</t>
   </si>
   <si>
+    <t>الأسئلة الشائعة</t>
+  </si>
+  <si>
     <t>privacy_policy</t>
   </si>
   <si>
     <t>Privacy policy</t>
   </si>
   <si>
+    <t>سياسة الخصوصية</t>
+  </si>
+  <si>
+    <t>Datenschutz</t>
+  </si>
+  <si>
     <t>terms_conditions</t>
   </si>
   <si>
     <t>Terms &amp; conditions</t>
   </si>
   <si>
+    <t>شروط الإستخدام</t>
+  </si>
+  <si>
+    <t>Bedingungen und Konditionen</t>
+  </si>
+  <si>
     <t>about_app</t>
   </si>
   <si>
     <t>About app</t>
   </si>
   <si>
+    <t>حول التطبيق</t>
+  </si>
+  <si>
+    <t>Über die App</t>
+  </si>
+  <si>
     <t>redeem_gifts</t>
   </si>
   <si>
-    <t>Click to buy a gift’s cards</t>
+    <t>Click to redeem gift’s cards</t>
+  </si>
+  <si>
+    <t>انقر هنا لطلب بطاقات الهدايا</t>
+  </si>
+  <si>
+    <t>Klicken Sie zum Einlösen von Geschenkkarten</t>
   </si>
   <si>
     <t>referrals</t>
@@ -274,478 +458,988 @@
     <t>Referrals</t>
   </si>
   <si>
+    <t>الدعوات</t>
+  </si>
+  <si>
+    <t>Freundschaftswerbung</t>
+  </si>
+  <si>
+    <t>refers_coins</t>
+  </si>
+  <si>
+    <t>Refer coins</t>
+  </si>
+  <si>
+    <t>نقاط الدعوات</t>
+  </si>
+  <si>
+    <t>Münzen beziehen</t>
+  </si>
+  <si>
+    <t>collect_gift_coins</t>
+  </si>
+  <si>
+    <t>Collect gift’s coins</t>
+  </si>
+  <si>
+    <t>اجمع المزيد من النقاط</t>
+  </si>
+  <si>
+    <t>Geschenkmünzen sammeln</t>
+  </si>
+  <si>
+    <t>refer_hint</t>
+  </si>
+  <si>
+    <t>Invite friends and get 10% of the points that thay collect.</t>
+  </si>
+  <si>
+    <t>قم بدعوة اصدقائك و احصل على 10٪ من النقاط التي يجمعونها.</t>
+  </si>
+  <si>
+    <t>Laden Sie Freunde ein und erhalten Sie 10% der gesammelten Punkte.</t>
+  </si>
+  <si>
+    <t>no_winners_today</t>
+  </si>
+  <si>
+    <t>No winners today yet</t>
+  </si>
+  <si>
+    <t>لا يوجد رابحين اليوم بعد</t>
+  </si>
+  <si>
+    <t>Heute noch keine Gewinner</t>
+  </si>
+  <si>
+    <t>coins</t>
+  </si>
+  <si>
+    <t>النقاط</t>
+  </si>
+  <si>
+    <t>Münzen</t>
+  </si>
+  <si>
+    <t>filter_date</t>
+  </si>
+  <si>
+    <t>Filter by date</t>
+  </si>
+  <si>
+    <t>تصفية حسب التاريخ</t>
+  </si>
+  <si>
+    <t>Nach Datum filtern</t>
+  </si>
+  <si>
+    <t>empty_play_time</t>
+  </si>
+  <si>
+    <t>There is No Playtime history yet</t>
+  </si>
+  <si>
+    <t>لا يوجد سجل لعب بعد</t>
+  </si>
+  <si>
+    <t>Es gibt noch keinen Spielzeitverlauf</t>
+  </si>
+  <si>
+    <t>play_game_now</t>
+  </si>
+  <si>
+    <t>Play game now</t>
+  </si>
+  <si>
+    <t>اللعب الان</t>
+  </si>
+  <si>
+    <t>Spiel jetzt spielen</t>
+  </si>
+  <si>
+    <t>dark_mode</t>
+  </si>
+  <si>
+    <t>Dark mode</t>
+  </si>
+  <si>
+    <t>الوضع الليلي</t>
+  </si>
+  <si>
+    <t>Dunkler Modus</t>
+  </si>
+  <si>
+    <t>dark_mode_subtitle</t>
+  </si>
+  <si>
+    <t>Try new dark mode theme</t>
+  </si>
+  <si>
+    <t>جرب الوضع الليلي لتطبيق هدية</t>
+  </si>
+  <si>
+    <t>Neues Thema für den dunklen Modus ausprobieren</t>
+  </si>
+  <si>
+    <t>change_number</t>
+  </si>
+  <si>
+    <t>Change phone number</t>
+  </si>
+  <si>
+    <t>تغيير رقم الهاتف المسجل</t>
+  </si>
+  <si>
+    <t>Handynummer ändern</t>
+  </si>
+  <si>
+    <t>change_number_subtitle</t>
+  </si>
+  <si>
+    <t>Change your mobile phone number</t>
+  </si>
+  <si>
+    <t>تغيير رقم هاتفك</t>
+  </si>
+  <si>
+    <t>Ändern Sie Ihre Handynummer</t>
+  </si>
+  <si>
+    <t>common_questions_subtitle</t>
+  </si>
+  <si>
+    <t>A lot of popular questions...</t>
+  </si>
+  <si>
+    <t>كثير من الاسئلة اللتي قد تهمك</t>
+  </si>
+  <si>
+    <t>Eine Menge beliebter Fragen...</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>حذف</t>
+  </si>
+  <si>
+    <t>löschen</t>
+  </si>
+  <si>
+    <t>delete_account</t>
+  </si>
+  <si>
+    <t>Delete account</t>
+  </si>
+  <si>
+    <t>حذف حسابي</t>
+  </si>
+  <si>
+    <t>Konto löschen</t>
+  </si>
+  <si>
+    <t>delete_account_subtitle</t>
+  </si>
+  <si>
+    <t>All account data will be deleted</t>
+  </si>
+  <si>
+    <t>جميع بيانات الحساب سيتم حذفها</t>
+  </si>
+  <si>
+    <t>Alle Kontodaten werden gelöscht</t>
+  </si>
+  <si>
+    <t>delete_account_message</t>
+  </si>
+  <si>
+    <t>All your account data will be deleted including coins and gifts!</t>
+  </si>
+  <si>
+    <t>جميع بيانات حسابك سيتم حذفها متضمنة نقاطك وهداياك</t>
+  </si>
+  <si>
+    <t>Alle Ihre Kontodaten werden gelöscht, einschließlich Münzen und Geschenke!</t>
+  </si>
+  <si>
+    <t>enter_delete_reason</t>
+  </si>
+  <si>
+    <t>Please tell us the reason</t>
+  </si>
+  <si>
+    <t>رجاءً اخبرنا السبب</t>
+  </si>
+  <si>
+    <t>Bitte teilen Sie uns den Grund mit</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>الملف الشخصي</t>
+  </si>
+  <si>
+    <t>Profil</t>
+  </si>
+  <si>
+    <t>edit_profile</t>
+  </si>
+  <si>
+    <t>Edit profile</t>
+  </si>
+  <si>
+    <t>تعديل الملف الشخصي</t>
+  </si>
+  <si>
+    <t>Profil bearbeiten</t>
+  </si>
+  <si>
+    <t>birth_date_hint</t>
+  </si>
+  <si>
+    <t>Your date of birth</t>
+  </si>
+  <si>
+    <t>تاريخ مولدك</t>
+  </si>
+  <si>
+    <t>Dein Geburtsdatum</t>
+  </si>
+  <si>
+    <t>gender_hint</t>
+  </si>
+  <si>
+    <t>Your gender</t>
+  </si>
+  <si>
+    <t>جنسك</t>
+  </si>
+  <si>
+    <t>Dein Geschlecht</t>
+  </si>
+  <si>
+    <t>years_old</t>
+  </si>
+  <si>
+    <t>Years old</t>
+  </si>
+  <si>
+    <t>عمرك</t>
+  </si>
+  <si>
+    <t>Jahre alt</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>حفظ</t>
+  </si>
+  <si>
+    <t>Speichern</t>
+  </si>
+  <si>
+    <t>saved</t>
+  </si>
+  <si>
+    <t>Saved</t>
+  </si>
+  <si>
+    <t>تم الحفظ</t>
+  </si>
+  <si>
+    <t>Gespeicherte</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>إلغاء</t>
+  </si>
+  <si>
+    <t>kündigen</t>
+  </si>
+  <si>
     <t>copy_code</t>
   </si>
   <si>
-    <t>Refer a friend</t>
-  </si>
-  <si>
-    <t>collect_gift_coins</t>
-  </si>
-  <si>
-    <t>Collect gift’s coins</t>
-  </si>
-  <si>
-    <t>refer_hint</t>
-  </si>
-  <si>
-    <t>Invite friends and get 10% of the points that thay collect. more info</t>
-  </si>
-  <si>
-    <t>no_winners_today</t>
-  </si>
-  <si>
-    <t>No winners today yet</t>
-  </si>
-  <si>
-    <t>coins</t>
-  </si>
-  <si>
-    <t>filter_date</t>
-  </si>
-  <si>
-    <t>Filter by date</t>
-  </si>
-  <si>
-    <t>empty_play_time</t>
-  </si>
-  <si>
-    <t>There is No Playtime history yet</t>
-  </si>
-  <si>
-    <t>play_game_now</t>
-  </si>
-  <si>
-    <t>Play game now</t>
-  </si>
-  <si>
-    <t>dark_mode</t>
-  </si>
-  <si>
-    <t>Dark mode</t>
-  </si>
-  <si>
-    <t>dark_mode_subtitle</t>
-  </si>
-  <si>
-    <t>Try new dark mode theme</t>
-  </si>
-  <si>
-    <t>change_number</t>
-  </si>
-  <si>
-    <t>Change phone number</t>
-  </si>
-  <si>
-    <t>change_number_subtitle</t>
-  </si>
-  <si>
-    <t>Change your mobile phone number</t>
-  </si>
-  <si>
-    <t>common_questions_subtitle</t>
-  </si>
-  <si>
-    <t>A lot of popular questions...</t>
-  </si>
-  <si>
-    <t>delete</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
-    <t>delete_account</t>
-  </si>
-  <si>
-    <t>Delete account</t>
-  </si>
-  <si>
-    <t>delete_account_subtitle</t>
-  </si>
-  <si>
-    <t>All account data will be deleted</t>
-  </si>
-  <si>
-    <t>delete_account_message</t>
-  </si>
-  <si>
-    <t>All your account data will be deleted including coins and gifts!</t>
-  </si>
-  <si>
-    <t>enter_delete_reason</t>
-  </si>
-  <si>
-    <t>Please tell us the reason</t>
-  </si>
-  <si>
-    <t>edit_profile</t>
-  </si>
-  <si>
-    <t>Edit profile</t>
-  </si>
-  <si>
-    <t>birth_date_hint</t>
-  </si>
-  <si>
-    <t>Your date of birth</t>
-  </si>
-  <si>
-    <t>gender_hint</t>
-  </si>
-  <si>
-    <t>Your gender</t>
-  </si>
-  <si>
-    <t>years_old</t>
-  </si>
-  <si>
-    <t>Years old</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>saved</t>
-  </si>
-  <si>
-    <t>Saved</t>
-  </si>
-  <si>
-    <t>cancel</t>
-  </si>
-  <si>
     <t>Copy code</t>
   </si>
   <si>
+    <t>نسخ الرمز</t>
+  </si>
+  <si>
+    <t>Code kopieren</t>
+  </si>
+  <si>
     <t>copied</t>
   </si>
   <si>
     <t>Copied</t>
   </si>
   <si>
+    <t>تم النسخ</t>
+  </si>
+  <si>
+    <t>Kopiert</t>
+  </si>
+  <si>
     <t>approved</t>
   </si>
   <si>
     <t>Approved</t>
   </si>
   <si>
+    <t>تم الموافقة</t>
+  </si>
+  <si>
+    <t>Genehmigt</t>
+  </si>
+  <si>
     <t>pending</t>
   </si>
   <si>
     <t>Pending</t>
   </si>
   <si>
+    <t>قيد التحقق</t>
+  </si>
+  <si>
+    <t>Ausstehend</t>
+  </si>
+  <si>
     <t>rejected</t>
   </si>
   <si>
     <t>Rejected</t>
   </si>
   <si>
+    <t>تم الرفض</t>
+  </si>
+  <si>
+    <t>Abgelehnt</t>
+  </si>
+  <si>
     <t>error_try_again</t>
   </si>
   <si>
     <t>An error happend, Please try again later</t>
   </si>
   <si>
+    <t>حصل خطأ,الرجاء المحاولة لاحقاً</t>
+  </si>
+  <si>
+    <t>Es ist ein Fehler aufgetreten, bitte versuchen Sie es später noch einmal</t>
+  </si>
+  <si>
     <t>chat_field_hint</t>
   </si>
   <si>
     <t>Type a message</t>
   </si>
   <si>
+    <t>اكتب رسالة</t>
+  </si>
+  <si>
+    <t>Geben Sie eine Nachricht ein</t>
+  </si>
+  <si>
     <t>no_common_questions</t>
   </si>
   <si>
     <t>No FAQ in the meaning time, Plaese come back later</t>
   </si>
   <si>
+    <t>لا أسئلة شائعة حاليا, عد لاحقاً عندما يتم إضافتها</t>
+  </si>
+  <si>
+    <t>Keine FAQ in der Bedeutung Zeit, Plaese kommen wieder später</t>
+  </si>
+  <si>
     <t>gifts_cards</t>
   </si>
   <si>
     <t>Gift’s Cards</t>
   </si>
   <si>
+    <t>بطاقات الهدايا</t>
+  </si>
+  <si>
+    <t>Geschenk-Karten</t>
+  </si>
+  <si>
     <t>empty_gift_list</t>
   </si>
   <si>
     <t>No gifts for the selected type at the moment</t>
   </si>
   <si>
+    <t>لا يوجد هدايا من هذا الصنف حالياً</t>
+  </si>
+  <si>
+    <t>Keine Geschenke für den ausgewählten Typ im Moment</t>
+  </si>
+  <si>
     <t>category_type</t>
   </si>
   <si>
     <t>Category type</t>
   </si>
   <si>
+    <t>نوغ الصنف</t>
+  </si>
+  <si>
+    <t>Kategorie Typ</t>
+  </si>
+  <si>
     <t>charge</t>
   </si>
   <si>
     <t>PAYOUT</t>
   </si>
   <si>
+    <t>شحن</t>
+  </si>
+  <si>
+    <t>AUSZAHLUNG</t>
+  </si>
+  <si>
     <t>gift_it</t>
   </si>
   <si>
     <t>Gift it</t>
   </si>
   <si>
+    <t>اطلب الهدية</t>
+  </si>
+  <si>
+    <t>Schenken</t>
+  </si>
+  <si>
     <t>verification</t>
   </si>
   <si>
     <t>Verification</t>
   </si>
   <si>
+    <t>التَحَقّق</t>
+  </si>
+  <si>
+    <t>Verifizierung</t>
+  </si>
+  <si>
     <t>verification_hint</t>
   </si>
   <si>
     <t>Enter your mobile phone number to verify your account and you can get gifts</t>
   </si>
   <si>
+    <t>ادخل رقم هاتفك ليتم التحقق من حسابك ويصبح بإمكانك طلب الهدايا</t>
+  </si>
+  <si>
+    <t>Geben Sie Ihre Handynummer ein, um Ihr Konto zu verifizieren, und Sie können Geschenke erhalten</t>
+  </si>
+  <si>
     <t>your_phone_number</t>
   </si>
   <si>
     <t>Your phone number</t>
   </si>
   <si>
+    <t>رقم هاتفك</t>
+  </si>
+  <si>
+    <t>Ihre Handynummer</t>
+  </si>
+  <si>
     <t>invalid_number</t>
   </si>
   <si>
     <t>Invalid phone number</t>
   </si>
   <si>
+    <t>رقم الهاتف خاطئ</t>
+  </si>
+  <si>
+    <t>Ungültige Handynummer</t>
+  </si>
+  <si>
     <t>code_submitted_hint</t>
   </si>
   <si>
     <t>Your code has been submitted, you will receive a message with a code that must be entered below</t>
   </si>
   <si>
+    <t>تم إرسال الرمز الخاص بك ، ستتلقى رسالة تحتوي على رمز يجب إدخاله أدناه</t>
+  </si>
+  <si>
+    <t>Ihr Code wurde übermittelt, Sie erhalten eine Nachricht mit einem Code, den Sie unten eingeben müssen</t>
+  </si>
+  <si>
     <t>code_sent_to</t>
   </si>
   <si>
     <t>Code will be sent to</t>
   </si>
   <si>
+    <t>سيتم إرسال الرمز إلى</t>
+  </si>
+  <si>
+    <t>Der Code wird gesendet an</t>
+  </si>
+  <si>
     <t>no_gifts_history_yet</t>
   </si>
   <si>
     <t>There are No gift requests yet</t>
   </si>
   <si>
+    <t>لا توجد طلبات هدايا حتى الآن</t>
+  </si>
+  <si>
+    <t>Es sind noch keine Geschenkanfragen vorhanden</t>
+  </si>
+  <si>
     <t>attention</t>
   </si>
   <si>
     <t>Attention</t>
   </si>
   <si>
+    <t>انتباه</t>
+  </si>
+  <si>
+    <t>Achtung</t>
+  </si>
+  <si>
     <t>task_agreement</t>
   </si>
   <si>
     <t>Failure to perform the task may lead to banning of your account.</t>
   </si>
   <si>
+    <t>قد يؤدي عدم أداء المهمة إلى حظر حسابك.</t>
+  </si>
+  <si>
+    <t>Die Nichterfüllung der Aufgabe kann zur Sperrung Ihres Kontos führen.</t>
+  </si>
+  <si>
     <t>select_language</t>
   </si>
   <si>
     <t>Select your Language</t>
   </si>
   <si>
+    <t>اختر لغتك</t>
+  </si>
+  <si>
+    <t>Wählen Sie Ihre Sprache</t>
+  </si>
+  <si>
     <t>notifications</t>
   </si>
   <si>
     <t>Notifications</t>
   </si>
   <si>
+    <t>الإشعارات</t>
+  </si>
+  <si>
+    <t>Benachrichtigungen</t>
+  </si>
+  <si>
     <t>empty_notifications_list</t>
   </si>
   <si>
     <t>There are No Notification yet</t>
   </si>
   <si>
+    <t>لا يوجد اشعارات حتى الان</t>
+  </si>
+  <si>
+    <t>Es sind noch keine Benachrichtigungen vorhanden</t>
+  </si>
+  <si>
     <t>copy_referral_hint</t>
   </si>
   <si>
     <t>Click to share your referral code</t>
   </si>
   <si>
+    <t>انقر لمشاركة رمز الإحالة الخاص بك</t>
+  </si>
+  <si>
+    <t>Klicken Sie, um Ihren Empfehlungscode zu teilen</t>
+  </si>
+  <si>
     <t>enter_code</t>
   </si>
   <si>
     <t>Enter referral code</t>
   </si>
   <si>
+    <t>أدخل رمز الإحالة</t>
+  </si>
+  <si>
+    <t>Empfehlungscode eingeben</t>
+  </si>
+  <si>
     <t>enter_code_short</t>
   </si>
   <si>
     <t>Enter code</t>
   </si>
   <si>
+    <t>ادخل الرمز</t>
+  </si>
+  <si>
+    <t>Code eingeben</t>
+  </si>
+  <si>
     <t>no_code_short</t>
   </si>
   <si>
     <t>Don't have code</t>
   </si>
   <si>
+    <t>ليس لدي رمز</t>
+  </si>
+  <si>
+    <t>Ich habe keinen Code</t>
+  </si>
+  <si>
     <t>accepted_referral_code</t>
   </si>
   <si>
+    <t>Referral code has been accepted</t>
+  </si>
+  <si>
+    <t>تم قبول رمز الإحالة</t>
+  </si>
+  <si>
+    <t>Empfehlungscode wurde akzeptiert</t>
+  </si>
+  <si>
     <t>account_suspicious</t>
   </si>
   <si>
     <t>Your account has been BLOCKED due to illegal use of the app., if you think this is a mistake please contact us</t>
   </si>
   <si>
+    <t>تم حظر حسابك بسبب الاستخدام غير القانوني للتطبيق. ، إذا كنت تعتقد أن هذا خطأ ، فيرجى الاتصال بنا</t>
+  </si>
+  <si>
+    <t>Ihr Konto wurde wegen illegaler Nutzung der App gesperrt. Wenn Sie glauben, dass dies ein Fehler ist, kontaktieren Sie uns bitte.</t>
+  </si>
+  <si>
     <t>exit</t>
   </si>
   <si>
     <t>Exit</t>
   </si>
   <si>
+    <t>خروج</t>
+  </si>
+  <si>
+    <t>Beenden</t>
+  </si>
+  <si>
     <t>accept</t>
   </si>
   <si>
     <t>Accept</t>
   </si>
   <si>
+    <t>موافق</t>
+  </si>
+  <si>
+    <t>Akzeptieren</t>
+  </si>
+  <si>
     <t>request_already_added</t>
   </si>
   <si>
     <t>The request already exists</t>
   </si>
   <si>
+    <t>الطلب موجود بالفعل</t>
+  </si>
+  <si>
+    <t>Die Anfrage existiert bereits</t>
+  </si>
+  <si>
     <t>check_data_correct</t>
   </si>
   <si>
     <t>Make sure the data is correct then try again later</t>
   </si>
   <si>
+    <t>تأكد من صحة البيانات ثم حاول مرة أخرى لاحقًا</t>
+  </si>
+  <si>
+    <t>Vergewissern Sie sich, dass die Daten korrekt sind und versuchen Sie es später noch einmal</t>
+  </si>
+  <si>
     <t>invalid_data</t>
   </si>
   <si>
     <t>Make sure the data is correct</t>
   </si>
   <si>
+    <t>تأكد من صحة البيانات</t>
+  </si>
+  <si>
+    <t>Stellen Sie sicher, dass die Daten korrekt sind</t>
+  </si>
+  <si>
     <t>vpn_warning</t>
   </si>
   <si>
     <t>You can NOT use Gifts App with VPN connection</t>
   </si>
   <si>
+    <t>لا يمكنك استخدام تطبيق هدية مع اتصال VPN</t>
+  </si>
+  <si>
+    <t>Sie können die Gifts App NICHT mit einer VPN-Verbindung verwenden</t>
+  </si>
+  <si>
     <t>wrong_email_password</t>
   </si>
   <si>
     <t>Wrong email or password</t>
   </si>
   <si>
+    <t>بريد إلكتروني أو كلمة مرور خاطئة</t>
+  </si>
+  <si>
+    <t>Falsche E-Mail oder falsches Passwort</t>
+  </si>
+  <si>
     <t>account_block_message</t>
   </si>
   <si>
     <t>Your account has been BLOCKED, see the FAQ and contact us if you think this happened by mistake</t>
   </si>
   <si>
+    <t>تم حظر حسابك ، راجع الأسئلة الشائعة واتصل بنا إذا كنت تعتقد أن هذا حدث عن طريق الخطأ</t>
+  </si>
+  <si>
+    <t>Ihr Konto wurde gesperrt, siehe FAQ und kontaktieren Sie uns, wenn Sie glauben, dass dies versehentlich geschehen ist.</t>
+  </si>
+  <si>
     <t>account_exist_on_other_message</t>
   </si>
   <si>
     <t>It is not allowed to log in with different emails on one device, please log in with the same email that was registered with</t>
   </si>
   <si>
+    <t>لا يمكن استخدام ايميل مختلف على هذا الجهاز، الرجاء العودة للايميل الذي قمت بالتسجيل به</t>
+  </si>
+  <si>
+    <t>Es ist nicht erlaubt, sich mit verschiedenen E-Mail-Adressen auf einem Gerät anzumelden. Bitte melden Sie sich mit der gleichen E-Mail an, mit der Sie sich registriert haben.</t>
+  </si>
+  <si>
     <t>fill_required_info</t>
   </si>
   <si>
     <t>Please fill in required info</t>
   </si>
   <si>
+    <t>الرجاء ملء البيانات المطلوبة</t>
+  </si>
+  <si>
+    <t>Bitte füllen Sie die erforderlichen Informationen aus</t>
+  </si>
+  <si>
     <t>winners_count</t>
   </si>
   <si>
     <t>Winners count</t>
   </si>
   <si>
+    <t>عدد الرابحين</t>
+  </si>
+  <si>
+    <t>Anzahl der Gewinner</t>
+  </si>
+  <si>
     <t>not_original_app_version</t>
   </si>
   <si>
     <t>Sorry, this is a non-original version of the "Gifts App", please download from the App Store</t>
   </si>
   <si>
+    <t>هذه نسخة غير مصرح لها , الرجاء تحميل تطبيق هدية من متجر التطبيقات</t>
+  </si>
+  <si>
+    <t>Entschuldigung, dies ist eine nicht-originale Version der "Gifts App", bitte laden Sie sie aus dem App Store herunter</t>
+  </si>
+  <si>
     <t>allow_storage_permission</t>
   </si>
   <si>
     <t>Storage permission not permitted</t>
   </si>
   <si>
+    <t>يرجى قبول صلاحيات التخزين أولاً</t>
+  </si>
+  <si>
+    <t>Speichererlaubnis nicht erlaubt</t>
+  </si>
+  <si>
     <t>emulator_prevented</t>
   </si>
   <si>
     <t>app can't be installed on an emulator device</t>
   </si>
   <si>
+    <t>لا يمكن تثبيت التطبيق على جهاز محاكي</t>
+  </si>
+  <si>
+    <t>Die App kann nicht auf einem Emulator-Gerät installiert werden</t>
+  </si>
+  <si>
     <t>account_block_duplicate</t>
   </si>
   <si>
     <t>This account has been banned, this is a modified version of the gifts App, please install the app from the app store</t>
   </si>
   <si>
+    <t>لقد تم ايقاف حسابك, يمكنك الحصول على تطبيق هدية من الحساب الرسمي في متجر التطبيقات فقط</t>
+  </si>
+  <si>
+    <t>Dieses Konto wurde gesperrt, dies ist eine modifizierte Version der Geschenke-App, bitte installieren Sie die App aus dem App Store</t>
+  </si>
+  <si>
     <t>update_available</t>
   </si>
   <si>
     <t>New version is available, Please update</t>
   </si>
   <si>
+    <t>الرجاء تحديث تطبيق هدية</t>
+  </si>
+  <si>
+    <t>Neue Version ist verfügbar, bitte aktualisieren</t>
+  </si>
+  <si>
     <t>claim_delay</t>
   </si>
   <si>
     <t>These Coins will be added to your balance after you open a game and get its points</t>
   </si>
   <si>
+    <t>سيتم اضافة هذه النقاط الى رصيدك بعد ان تفتح لعبة و تحصل على نقاطها</t>
+  </si>
+  <si>
+    <t>Diese Coins werden deinem Guthaben hinzugefügt, nachdem du ein Spiel geöffnet und dessen Punkte erhalten hast</t>
+  </si>
+  <si>
     <t>gift_request_registered</t>
   </si>
   <si>
     <t>Your request will be processed within a maximum 7 days .. Please, follow the gifts history</t>
   </si>
   <si>
+    <t>تم تسجيل طلبك بنجاح, بحسب عدد الطلبات قد يستغرق التحقق من طلبك مدة لا تتجاوز 7 ايام. رجاءً تابع طلبك في صفحة سجل الهدايا</t>
+  </si>
+  <si>
+    <t>Deine Anfrage wird innerhalb von maximal 7 Tagen bearbeitet. Bitte verfolge die Geschenke-Historie</t>
+  </si>
+  <si>
     <t>not_enough_balance</t>
   </si>
   <si>
     <t>There is not enough coins in your account</t>
   </si>
   <si>
+    <t>لا يوجد رصيد كاف</t>
+  </si>
+  <si>
+    <t>Es gibt nicht genug Münzen auf Ihrem Konto</t>
+  </si>
+  <si>
     <t>no_cards_available</t>
   </si>
   <si>
     <t>There are no cards currently available for the requested card</t>
   </si>
   <si>
+    <t>لا يوجد بطاقات متوفرة حالياً للبطاقة المطلوبة</t>
+  </si>
+  <si>
+    <t>Es sind derzeit keine Karten für die angeforderte Karte verfügbar</t>
+  </si>
+  <si>
     <t>changed_number_error</t>
   </si>
   <si>
     <t>Your registered number is</t>
   </si>
   <si>
+    <t>رقمك المسجل هو</t>
+  </si>
+  <si>
+    <t>Ihre registrierte Nummer ist</t>
+  </si>
+  <si>
     <t>gaid_denied_message</t>
   </si>
   <si>
     <t>Please permit the ads tracking permission for this app to verify your account validity</t>
   </si>
   <si>
+    <t>يجب منح التطبيق اذن تتبع تطبيقات الالعاب ليتم حساب الوقت و ارسال النقاط لرصيدك</t>
+  </si>
+  <si>
+    <t>Bitte erlauben Sie die Werbeverfolgung für diese App, um die Gültigkeit Ihres Kontos zu überprüfen</t>
+  </si>
+  <si>
     <t>rate_our_app</t>
   </si>
   <si>
     <t>Rate Gifts App</t>
   </si>
   <si>
+    <t>قيم تطبيق هدية</t>
+  </si>
+  <si>
+    <t>Gifts App bewerten</t>
+  </si>
+  <si>
     <t>exit_app</t>
   </si>
   <si>
     <t>Exit Gifts App?</t>
   </si>
   <si>
+    <t>هل تريد اغلاق تطبيق هدية؟</t>
+  </si>
+  <si>
+    <t>Gifts App beenden?</t>
+  </si>
+  <si>
     <t>complete_profile_message</t>
   </si>
   <si>
     <t>Please complete your profile info</t>
+  </si>
+  <si>
+    <t>الرجاء ملء البيانات المطلوبة اولاً</t>
+  </si>
+  <si>
+    <t>Bitte vervollständigen Sie Ihre Profilinformationen</t>
   </si>
   <si>
     <t>review_app_message</t>
@@ -755,53 +1449,586 @@
  please rate Gifts App</t>
   </si>
   <si>
+    <t>هل اعجبك تطبيق هدية؟ 
+ قم بتقييم التطبيق الان</t>
+  </si>
+  <si>
+    <t>Genießen Sie es, Zeit mit uns zu verbringen?
+ Bitte bewerten Sie Gifts App</t>
+  </si>
+  <si>
     <t>exit_gift_request</t>
   </si>
   <si>
     <t>Exiting will cancel the gift request</t>
   </si>
   <si>
+    <t>سيتم الغاء طلب الهدية! لا تقلق لن يتم خصم نقاط</t>
+  </si>
+  <si>
+    <t>Beim Beenden wird die Geschenkanfrage abgebrochen</t>
+  </si>
+  <si>
     <t>competition_cost</t>
   </si>
   <si>
     <t>Entering fee</t>
   </si>
   <si>
+    <t>كلفة الاشتراك</t>
+  </si>
+  <si>
+    <t>Eingabe der Gebühr</t>
+  </si>
+  <si>
     <t>finish_task_confirm</t>
   </si>
   <si>
     <t>Did you perform the task?</t>
   </si>
   <si>
+    <t>هل قمت بتنفيذ المهمة ؟</t>
+  </si>
+  <si>
+    <t>Haben Sie die Aufgabe erfüllt?</t>
+  </si>
+  <si>
     <t>no_account_in_task_link</t>
   </si>
   <si>
     <t>I have no account to do the task!</t>
   </si>
   <si>
+    <t>لا املك حساب في هذا الموقع</t>
+  </si>
+  <si>
+    <t>Ich habe kein Konto, um die Aufgabe zu erledigen!</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>نعم</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
     <t>get_more_points_now</t>
   </si>
   <si>
     <t>Get more coins now?</t>
   </si>
   <si>
+    <t>احصل على المزيد من النقاط الآن؟</t>
+  </si>
+  <si>
+    <t>Jetzt mehr Münzen erhalten?</t>
+  </si>
+  <si>
     <t>copy_share_link_hint</t>
   </si>
   <si>
     <t>Copy the referral Link and share it on Facebook, YouTube and Instagram to get more coins and be on the list</t>
+  </si>
+  <si>
+    <t>انسخ رابط الدعوات و شاركه على حساباتك في فيسبوك و انستغرام و الواتس اب تكون في الصدارة والربح من نقاط اصدقائك</t>
+  </si>
+  <si>
+    <t>Kopiere den Empfehlungslink und teile ihn auf Facebook, YouTube und Instagram, um mehr Münzen zu erhalten und auf der Liste zu stehen.</t>
+  </si>
+  <si>
+    <t>allTime</t>
+  </si>
+  <si>
+    <t>All Time</t>
+  </si>
+  <si>
+    <t>جميع السجلات</t>
+  </si>
+  <si>
+    <t>Alle Zeiten</t>
+  </si>
+  <si>
+    <t>lastWeek</t>
+  </si>
+  <si>
+    <t>Last Week</t>
+  </si>
+  <si>
+    <t>الأسبوع الماضي</t>
+  </si>
+  <si>
+    <t>Letzte Woche</t>
+  </si>
+  <si>
+    <t>lastMonth</t>
+  </si>
+  <si>
+    <t>Last Month</t>
+  </si>
+  <si>
+    <t>الشهر الماضي</t>
+  </si>
+  <si>
+    <t>Letzter Monat</t>
+  </si>
+  <si>
+    <t>friend_referrals</t>
+  </si>
+  <si>
+    <t>Friend referrals</t>
+  </si>
+  <si>
+    <t>إحالات الأصدقاء</t>
+  </si>
+  <si>
+    <t>Freundschaftswerbungen</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>ذكر</t>
+  </si>
+  <si>
+    <t>Männlich</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>أنثى</t>
+  </si>
+  <si>
+    <t>Weiblich</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Unselected</t>
+  </si>
+  <si>
+    <t>غير محدد</t>
+  </si>
+  <si>
+    <t>Ungewählt</t>
+  </si>
+  <si>
+    <t>share_referral_message</t>
+  </si>
+  <si>
+    <t>"Gifts App" rewards you CASH.
+I Got $10 in less than an hour only!
+You too can do it .. what are you waiting for !
+Download NOW.</t>
+  </si>
+  <si>
+    <t>انا ربحت من تطبيق هدية بسهولة, انت كمان تقدر تربح. 
+ هاد تطبيق بيطلب منك تلعب بلعبة و بيدفعلك كاش او بطاقات جوجل و ماستر كارد و نقاط تيك توك و كتير هدايا رائعة.
+ لا تتردد حمل التطبيق و ابدأ بالربح.</t>
+  </si>
+  <si>
+    <t>"Gifts App" belohnt dich mit CASH.
+Ich habe $10 in weniger als einer Stunde erhalten!
+Du kannst es auch tun ... worauf wartest du noch!
+Download NOW.</t>
+  </si>
+  <si>
+    <t>share_referral_message2</t>
+  </si>
+  <si>
+    <t>Use referral link</t>
+  </si>
+  <si>
+    <t>رابط الدعوة</t>
+  </si>
+  <si>
+    <t>Empfehlungslink verwenden</t>
+  </si>
+  <si>
+    <t>share_referral_message2_with_link</t>
+  </si>
+  <si>
+    <t>Download the app from the link</t>
+  </si>
+  <si>
+    <t>حمل تطبيق هدية من الرابط</t>
+  </si>
+  <si>
+    <t>Laden Sie die App über den Link</t>
+  </si>
+  <si>
+    <t>share_referral_message3</t>
+  </si>
+  <si>
+    <t>to get 500 Coins.</t>
+  </si>
+  <si>
+    <t>و اربح 500 نقطة مجانية</t>
+  </si>
+  <si>
+    <t>um 500 Münzen zu erhalten.</t>
+  </si>
+  <si>
+    <t>referral_code</t>
+  </si>
+  <si>
+    <t>Referrral code</t>
+  </si>
+  <si>
+    <t>رمز الإحالة</t>
+  </si>
+  <si>
+    <t>Empfehlungscode</t>
+  </si>
+  <si>
+    <t>more_info</t>
+  </si>
+  <si>
+    <t>More info</t>
+  </si>
+  <si>
+    <t>المزيد من التفاصيل</t>
+  </si>
+  <si>
+    <t>Mehr Infos</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>نسخة</t>
+  </si>
+  <si>
+    <t>about_app_short_description</t>
+  </si>
+  <si>
+    <t>in few lines description of the app itself and what it does</t>
+  </si>
+  <si>
+    <t>support_chat_hint</t>
+  </si>
+  <si>
+    <t>Welcome to the tech support of "Gifts App".
+ please send us What is the problem that appeared to you? and we will reach to you ASAP.</t>
+  </si>
+  <si>
+    <t>اهلا بك في الدعم الفني لتطبيق هدية 
+ الرجاء شرح المشكلة التي تواجهها و سنقوم بالرد عليك بأسرع وقت ممكن.</t>
+  </si>
+  <si>
+    <t>Willkommen beim technischen Support der "Gifts App".
+Bitte sende uns, was das Problem, das bei dir aufgetreten ist?
+und wir werden uns so schnell wie möglich an dir wenden.</t>
+  </si>
+  <si>
+    <t>see_all</t>
+  </si>
+  <si>
+    <t>See all</t>
+  </si>
+  <si>
+    <t>عرض الكل</t>
+  </si>
+  <si>
+    <t>Alle anzeigen</t>
+  </si>
+  <si>
+    <t>repeated_phone_number_warning</t>
+  </si>
+  <si>
+    <t>You have used this phone number before so it can not be used again</t>
+  </si>
+  <si>
+    <t>لقد استخدمت رقم الهاتف هذا من قبل لذا لا يمكن استخدامه مرة أخرى</t>
+  </si>
+  <si>
+    <t>Sie haben diese Rufnummer schon einmal benutzt, daher kann sie nicht erneut verwendet werden</t>
+  </si>
+  <si>
+    <t>number_exists</t>
+  </si>
+  <si>
+    <t>This number already exists</t>
+  </si>
+  <si>
+    <t>هذا الرقم موجود بالفعل</t>
+  </si>
+  <si>
+    <t>Diese Nummer existiert bereits</t>
+  </si>
+  <si>
+    <t>number_used_by_other</t>
+  </si>
+  <si>
+    <t>This number is used by another user, you have to use another one</t>
+  </si>
+  <si>
+    <t>هذا الرقم مستخدم من قبل مستخدم آخر ، يجب عليك استخدام رقم آخر</t>
+  </si>
+  <si>
+    <t>Diese Nummer wird von einem anderen Benutzer verwendet, Sie müssen eine andere Nummer verwenden</t>
+  </si>
+  <si>
+    <t>phone_number_warning</t>
+  </si>
+  <si>
+    <t>When you change number, you can’t use it in future</t>
+  </si>
+  <si>
+    <t>عندما تقوم بتغيير رقمك, لا يمكنك استخدامه في المستقبل</t>
+  </si>
+  <si>
+    <t>Wenn Sie die Nummer ändern, können Sie sie in Zukunft nicht mehr verwenden</t>
+  </si>
+  <si>
+    <t>old_phone_number</t>
+  </si>
+  <si>
+    <t>Old number</t>
+  </si>
+  <si>
+    <t>الرقم القديم</t>
+  </si>
+  <si>
+    <t>Alte Nummer</t>
+  </si>
+  <si>
+    <t>new_phone_number</t>
+  </si>
+  <si>
+    <t>New Number</t>
+  </si>
+  <si>
+    <t>الرقم الجديد</t>
+  </si>
+  <si>
+    <t>Neue Nummer</t>
+  </si>
+  <si>
+    <t>good_message</t>
+  </si>
+  <si>
+    <t>All things is great now</t>
+  </si>
+  <si>
+    <t>كل شيئ ممتاز الان</t>
+  </si>
+  <si>
+    <t>Jetzt ist alles super</t>
+  </si>
+  <si>
+    <t>verified_number_message</t>
+  </si>
+  <si>
+    <t>You can get your gifts now smoothly!</t>
+  </si>
+  <si>
+    <t>يمكنك طلب الهدايا بسهولة!</t>
+  </si>
+  <si>
+    <t>Sie können Ihre Geschenke jetzt reibungslos erhalten!</t>
+  </si>
+  <si>
+    <t>wrong_sms_code</t>
+  </si>
+  <si>
+    <t>The code you just entered is not valid</t>
+  </si>
+  <si>
+    <t>الرمز الذي أدخلته غير صالح</t>
+  </si>
+  <si>
+    <t>Der Code, den Sie gerade eingegeben haben, ist nicht gültig</t>
+  </si>
+  <si>
+    <t>check_number</t>
+  </si>
+  <si>
+    <t>Is this still your number?</t>
+  </si>
+  <si>
+    <t>هل لا يزال هذا رقمك؟</t>
+  </si>
+  <si>
+    <t>Ist dies noch Ihre Nummer?</t>
+  </si>
+  <si>
+    <t>auto_enter_phone_number_hint</t>
+  </si>
+  <si>
+    <t>We will send a verification code to this number to verify its you</t>
+  </si>
+  <si>
+    <t>سوف نرسل رمز تفعيل لهذا الرقم لنتحقق أنه أنت</t>
+  </si>
+  <si>
+    <t>Wir werden einen Verifizierungscode an diese Nummer senden, um zu überprüfen, ob Sie es sind.</t>
+  </si>
+  <si>
+    <t>earn_coins</t>
+  </si>
+  <si>
+    <t>Coin earnings</t>
+  </si>
+  <si>
+    <t>تجميع النقاط</t>
+  </si>
+  <si>
+    <t>Münzeinnahmen</t>
+  </si>
+  <si>
+    <t>top_users</t>
+  </si>
+  <si>
+    <t>Top users</t>
+  </si>
+  <si>
+    <t>المستخدمين التوب</t>
+  </si>
+  <si>
+    <t>Top-Benutzer</t>
+  </si>
+  <si>
+    <t>wrong_phone_range</t>
+  </si>
+  <si>
+    <t>Phone number not allowed</t>
+  </si>
+  <si>
+    <t>رقم الهاتف غير مسموح به</t>
+  </si>
+  <si>
+    <t>Rufnummer nicht erlaubt</t>
+  </si>
+  <si>
+    <t>wrong_phone_range_sub</t>
+  </si>
+  <si>
+    <t>You can not use a phone number from other than your country</t>
+  </si>
+  <si>
+    <t>لا يمكنك استخدام رقم هاتف من خارج بلدك</t>
+  </si>
+  <si>
+    <t>Sie können keine Telefonnummer aus einem anderen Land als Ihrem Land verwenden</t>
+  </si>
+  <si>
+    <t>send_image_hint</t>
+  </si>
+  <si>
+    <t>Send this image?</t>
+  </si>
+  <si>
+    <t>إرسال هذه الصورة؟</t>
+  </si>
+  <si>
+    <t>Dieses Bild senden?</t>
+  </si>
+  <si>
+    <t>play_button_tutorial_title</t>
+  </si>
+  <si>
+    <t>Play time button</t>
+  </si>
+  <si>
+    <t>زر وقت اللعب</t>
+  </si>
+  <si>
+    <t>Schaltfläche "Spielzeit</t>
+  </si>
+  <si>
+    <t>play_button_tutorial_subtitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Click the play time button To start collecting points and winning gifts</t>
+  </si>
+  <si>
+    <t>انقر فوق زر وقت اللعب لبدء جمع النقاط والفوز بالهدايا</t>
+  </si>
+  <si>
+    <t>Klicken Sie auf die Schaltfläche "Spielzeit", um Punkte zu sammeln und Geschenke zu gewinnen</t>
+  </si>
+  <si>
+    <t>redeem_tutorial_title</t>
+  </si>
+  <si>
+    <t>Redeem gifts here</t>
+  </si>
+  <si>
+    <t>اطلب هديتك من هنا</t>
+  </si>
+  <si>
+    <t>Geschenke hier einlösen</t>
+  </si>
+  <si>
+    <t>redeem_tutorial_subtitle</t>
+  </si>
+  <si>
+    <t>Got enouph coins? you can requests your gifts from here</t>
+  </si>
+  <si>
+    <t>هل حصلت على نقاط كافية؟ يمكنك طلب هداياك من هنا</t>
+  </si>
+  <si>
+    <t>Hast du genug Münzen? Du kannst deine Geschenke hier anfordern</t>
+  </si>
+  <si>
+    <t>cant_open_store_link</t>
+  </si>
+  <si>
+    <t>Could not open the apps store on your device</t>
+  </si>
+  <si>
+    <t>تعذر فتح متجر التطبيقات على جهازك</t>
+  </si>
+  <si>
+    <t>Der App-Store konnte auf deinem Gerät nicht geöffnet werden</t>
+  </si>
+  <si>
+    <t>update_dialog_title</t>
+  </si>
+  <si>
+    <t>Great news!</t>
+  </si>
+  <si>
+    <t>أخبار رائعة!</t>
+  </si>
+  <si>
+    <t>Tolle Neuigkeiten!</t>
+  </si>
+  <si>
+    <t>update_app</t>
+  </si>
+  <si>
+    <t>Update app</t>
+  </si>
+  <si>
+    <t>تحديث التطبيق</t>
+  </si>
+  <si>
+    <t>App aktualisieren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -809,6 +2036,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -828,7 +2061,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -836,6 +2069,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1094,1020 +2330,2311 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>80</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>84</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>88</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>92</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>96</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>100</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>103</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>107</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>111</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>72</v>
+        <v>115</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>119</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>76</v>
+        <v>123</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>126</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>130</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>134</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>84</v>
+        <v>138</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>86</v>
+        <v>142</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>88</v>
+        <v>146</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>90</v>
+        <v>150</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>92</v>
+        <v>154</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>158</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>95</v>
+        <v>161</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>96</v>
+        <v>164</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>97</v>
+        <v>165</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>99</v>
+        <v>169</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>101</v>
+        <v>173</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>102</v>
+        <v>176</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>103</v>
+        <v>177</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>104</v>
+        <v>180</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>181</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>107</v>
+        <v>185</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>109</v>
+        <v>189</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>110</v>
+        <v>192</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>111</v>
+        <v>193</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>112</v>
+        <v>196</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>113</v>
+        <v>197</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>114</v>
+        <v>200</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>115</v>
+        <v>201</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>117</v>
+        <v>205</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>118</v>
+        <v>208</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>119</v>
+        <v>209</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>120</v>
+        <v>212</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>121</v>
+        <v>213</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>122</v>
+        <v>216</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>123</v>
+        <v>217</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>124</v>
+        <v>220</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>125</v>
+        <v>221</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>126</v>
+        <v>224</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>127</v>
+        <v>225</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>128</v>
+        <v>228</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>129</v>
+        <v>229</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>130</v>
+        <v>232</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>131</v>
+        <v>233</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>132</v>
+        <v>236</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>133</v>
+        <v>237</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>134</v>
+        <v>240</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>134</v>
+        <v>241</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>87</v>
+        <v>244</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>244</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>137</v>
+        <v>248</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>139</v>
+        <v>252</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>140</v>
+        <v>255</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>141</v>
+        <v>256</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>142</v>
+        <v>259</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>143</v>
+        <v>260</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>144</v>
+        <v>263</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>145</v>
+        <v>264</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>146</v>
+        <v>267</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>147</v>
+        <v>268</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>148</v>
+        <v>271</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>149</v>
+        <v>272</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>150</v>
+        <v>275</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>151</v>
+        <v>276</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>152</v>
+        <v>279</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>153</v>
+        <v>280</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>154</v>
+        <v>283</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>155</v>
+        <v>284</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>156</v>
+        <v>287</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>157</v>
+        <v>288</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>158</v>
+        <v>291</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>159</v>
+        <v>292</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>160</v>
+        <v>295</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>161</v>
+        <v>296</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>162</v>
+        <v>299</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>163</v>
+        <v>300</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>164</v>
+        <v>303</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>165</v>
+        <v>304</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>166</v>
+        <v>307</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>167</v>
+        <v>308</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>168</v>
+        <v>311</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>169</v>
+        <v>312</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>170</v>
+        <v>315</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>171</v>
+        <v>316</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>172</v>
+        <v>319</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>173</v>
+        <v>320</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>174</v>
+        <v>323</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>175</v>
+        <v>324</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>176</v>
+        <v>327</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>177</v>
+        <v>328</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>178</v>
+        <v>331</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>179</v>
+        <v>332</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>180</v>
+        <v>335</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>181</v>
+        <v>336</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>182</v>
+        <v>339</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>183</v>
+        <v>340</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>184</v>
+        <v>343</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>185</v>
+        <v>344</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>186</v>
+        <v>347</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>187</v>
+        <v>348</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>188</v>
+        <v>351</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>189</v>
+        <v>352</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>190</v>
+        <v>355</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>191</v>
+        <v>356</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>192</v>
+        <v>359</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>192</v>
+        <v>360</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>193</v>
+        <v>363</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>194</v>
+        <v>364</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>195</v>
+        <v>367</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>196</v>
+        <v>368</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>197</v>
+        <v>371</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>198</v>
+        <v>372</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>199</v>
+        <v>375</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>200</v>
+        <v>376</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>201</v>
+        <v>379</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>202</v>
+        <v>380</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>203</v>
+        <v>383</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>204</v>
+        <v>384</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>205</v>
+        <v>387</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>206</v>
+        <v>388</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>207</v>
+        <v>391</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>208</v>
+        <v>392</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>209</v>
+        <v>395</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>210</v>
+        <v>396</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>211</v>
+        <v>399</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>212</v>
+        <v>400</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>213</v>
+        <v>403</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>214</v>
+        <v>404</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>215</v>
+        <v>407</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>216</v>
+        <v>408</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>217</v>
+        <v>411</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>218</v>
+        <v>412</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>219</v>
+        <v>415</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>220</v>
+        <v>416</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>221</v>
+        <v>419</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>222</v>
+        <v>420</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>223</v>
+        <v>423</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>224</v>
+        <v>424</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>225</v>
+        <v>427</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>226</v>
+        <v>428</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>227</v>
+        <v>431</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>228</v>
+        <v>432</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>229</v>
+        <v>435</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>230</v>
+        <v>436</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>231</v>
+        <v>439</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>232</v>
+        <v>440</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>233</v>
+        <v>443</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>234</v>
+        <v>444</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>235</v>
+        <v>447</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>236</v>
+        <v>448</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
-        <v>237</v>
+        <v>451</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>238</v>
+        <v>452</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>239</v>
+        <v>455</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>240</v>
+        <v>456</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>241</v>
+        <v>459</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>242</v>
+        <v>460</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
-        <v>243</v>
+        <v>463</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>244</v>
+        <v>464</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>245</v>
+        <v>467</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>246</v>
+        <v>468</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>247</v>
+        <v>471</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>248</v>
+        <v>472</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>249</v>
+        <v>475</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>250</v>
+        <v>476</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>251</v>
+        <v>479</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>252</v>
+        <v>480</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>253</v>
+        <v>483</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>254</v>
+        <v>484</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>255</v>
+        <v>487</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>256</v>
+        <v>488</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>257</v>
+        <v>491</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>258</v>
+        <v>492</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>259</v>
+        <v>495</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>260</v>
-      </c>
+        <v>496</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169">
+      <c r="D169" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>